<commit_message>
Ajustei o relatorio de estoque
</commit_message>
<xml_diff>
--- a/relatorio_diario.xlsx
+++ b/relatorio_diario.xlsx
@@ -473,7 +473,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>23/06/2025</t>
+          <t>26/06/2025</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -483,22 +483,22 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>120.99 kg (8 cx)</t>
+          <t>114.77 kg (8 cx)</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>128.25 kg</t>
+          <t>118.97 kg</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>120.71 kg</t>
+          <t>133.59 kg</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>1 dia</t>
+          <t>2 dias</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">

</xml_diff>